<commit_message>
Add Lab 9 Task 3
</commit_message>
<xml_diff>
--- a/lab9/task.xlsx
+++ b/lab9/task.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -126,6 +126,85 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Распределение зарплаты по отделам</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet'!$B$17:$B$19</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Sheet'!$E$17:$E$19</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>11</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -847,6 +926,9 @@
           <t>6684.78 руб.</t>
         </is>
       </c>
+      <c r="E17" t="n">
+        <v>6684.78</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" t="inlineStr">
@@ -859,6 +941,9 @@
           <t>7222.02 руб.</t>
         </is>
       </c>
+      <c r="E18" t="n">
+        <v>7222.02</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" t="inlineStr">
@@ -871,8 +956,12 @@
           <t>9000.00 руб.</t>
         </is>
       </c>
+      <c r="E19" t="n">
+        <v>9000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>